<commit_message>
Add Common Function test
</commit_message>
<xml_diff>
--- a/src/test/resources/templates/common-functions.xlsx
+++ b/src/test/resources/templates/common-functions.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17820" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="26865" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +29,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>RJ</author>
+    <author>bcsoft</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
@@ -43,22 +43,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>jx:area(lastCell="F6")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>jx:each(items="rows" var="r" lastCell="F4")</t>
+          <t>jx:area(lastCell="C7")</t>
         </r>
       </text>
     </comment>
@@ -67,81 +52,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Stage</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>YearMonth</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>DateTime</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Str</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>${num}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.format(date, 'yyyy/MM/dd')}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.format(datetime, 'yyyy/MM/dd HH:mm')}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.round(num, 2)}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.format(num, '#,###.00')}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${time}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.format(time, 'HH:mm')}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${datetime}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${date}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${str}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Origin Value (toString())</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Formatted Value</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>${fn.toInt(str)}</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>roundNumber</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>formatNumber</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>formatDateTime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>formatDate</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>formatTime</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>toInt</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Remark</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Generated Time：${ts}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${empty(r.remark) ? '[NONE]' : r.remark}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${fn.toInt(fn.format(r.yearMonth, 'yyyyMM'))}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${r.str}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Money</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${r.money}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${stageLabels[r.stage]}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Excel template test with some custom function</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>${fn.format(r.dateTime, 'yyyy-MM-dd HH:mm:ss')}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stage：${stage}, Search：${search?:'NONE'}</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Custom Functions: fn.format, fn.toInt</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="177" formatCode="\$#,##0.00;\-\$#,##0.00"/>
-  </numFmts>
-  <fonts count="10">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,41 +161,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF31859C"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -229,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -252,43 +219,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -296,20 +262,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -395,97 +358,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -754,99 +626,100 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="21.95" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="21.95" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" ht="21.95" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" ht="21.95" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="2" customFormat="1" ht="21.95" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="2" customFormat="1" ht="21.95" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="2" customFormat="1" ht="21.95" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="24" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" ht="24" customHeight="1">
-      <c r="A4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" ht="12" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="24" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="6" customFormat="1">
-      <c r="A8" s="6" t="s">
-        <v>15</v>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="63" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>